<commit_message>
Separated paid company options from user settings. Revised database mechanism.
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09826663-1563-4F9B-A80D-B66616BEC79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795F1212-C402-4125-8448-6ACA5ABD449F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
   <si>
     <t>Free</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Timelog - Make every second count</t>
+  </si>
+  <si>
+    <t>Can select multiples (15 or 30 minutes)</t>
   </si>
 </sst>
 </file>
@@ -469,42 +472,6 @@
   </cellStyleXfs>
   <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -524,27 +491,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -573,24 +519,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -603,10 +531,25 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -618,6 +561,108 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -627,53 +672,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,302 +1003,302 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C75CBC2-A4B4-4CDB-9F64-6654769FA256}">
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="18"/>
-    <col min="2" max="2" width="3.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="10.28515625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="64.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="3.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="10.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="64.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="72"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="17" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="7">
         <v>1</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="7">
         <v>5</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="7">
         <v>10</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="35" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="14">
         <v>0</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="14">
         <v>0</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="14">
         <v>2</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="14">
         <v>5</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="15" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="7">
         <v>0</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="7">
         <v>0</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="7">
         <v>5</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="7">
         <v>25</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="7">
         <v>1</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="7">
         <v>5</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="7">
         <v>10</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="7">
         <v>50</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="20"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="7">
         <v>1</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="7">
         <v>10</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="7">
         <v>20</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="20"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="8"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="7">
         <v>50</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="9">
         <v>100</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="20"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="7">
         <v>4</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="7">
         <v>50</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="20"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="8"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="15" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="19" t="s">
+      <c r="G15" s="30"/>
+      <c r="H15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="20"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="27"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="36" t="s">
+      <c r="B17" s="42"/>
+      <c r="C17" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="14">
         <v>1</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G17" s="14">
         <v>5</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="H17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="34"/>
+      <c r="I17" s="15"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="53"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1321,209 +1324,209 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8890EB03-9831-4A84-BAA4-07E57C463030}">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="30"/>
-    <col min="2" max="2" width="3.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.28515625" style="30" customWidth="1"/>
-    <col min="6" max="6" width="76.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="30"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.28515625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="76.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="38" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="44">
         <v>9.99</v>
       </c>
       <c r="E4" s="44"/>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="37" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="44">
         <v>5.99</v>
       </c>
       <c r="E5" s="44"/>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="37" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="18" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="44">
         <v>2.99</v>
       </c>
       <c r="E6" s="44"/>
-      <c r="F6" s="31"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="27"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="37" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="44">
         <v>9.99</v>
       </c>
       <c r="E8" s="44"/>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="37" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="44">
         <v>1.99</v>
       </c>
       <c r="E9" s="44"/>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="37" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="18" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="44">
         <v>0.99</v>
       </c>
       <c r="E10" s="44"/>
-      <c r="F10" s="31"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="37" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="44">
         <v>0.09</v>
       </c>
       <c r="E11" s="44"/>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="19" t="s">
+      <c r="B14" s="42"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="13">
         <v>2.99</v>
       </c>
-      <c r="F14" s="31" t="s">
-        <v>28</v>
+      <c r="F14" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="19" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="13">
         <v>5.99</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="19" t="s">
+      <c r="B16" s="42"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="13">
         <v>9.99</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="27"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="37" t="s">
+      <c r="B18" s="42"/>
+      <c r="C18" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="44">
@@ -1532,12 +1535,18 @@
       <c r="E18" s="44">
         <v>4.99</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="12" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:B18"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D8:E8"/>
@@ -1547,12 +1556,6 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1569,532 +1572,542 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="18"/>
-    <col min="2" max="2" width="3.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="68" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="68" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="68" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="29" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="68" customWidth="1"/>
-    <col min="12" max="12" width="64.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="3.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="27" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="27" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="27" customWidth="1"/>
+    <col min="12" max="12" width="64.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="72"/>
+      <c r="F2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="72"/>
+      <c r="J2" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="46" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="17" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="67" t="s">
+      <c r="I3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="67" t="s">
+      <c r="K3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="65">
+      <c r="D4" s="64"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="64">
         <v>2</v>
       </c>
-      <c r="G4" s="66"/>
-      <c r="H4" s="65">
+      <c r="G4" s="65"/>
+      <c r="H4" s="64">
         <v>2</v>
       </c>
-      <c r="I4" s="66"/>
-      <c r="J4" s="65">
+      <c r="I4" s="65"/>
+      <c r="J4" s="64">
         <v>1</v>
       </c>
-      <c r="K4" s="66"/>
-      <c r="L4" s="64"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="61"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="62"/>
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="14">
         <v>4</v>
       </c>
-      <c r="G5" s="48">
+      <c r="G5" s="23">
         <f>(F5-D5)*Prices!$D$4</f>
         <v>29.97</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="14">
         <v>9</v>
       </c>
-      <c r="I5" s="48">
+      <c r="I5" s="23">
         <f>(H5-F5)*Prices!$D$4</f>
         <v>49.95</v>
       </c>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="48">
+      <c r="K5" s="23">
         <f>2*I5/J$4</f>
         <v>99.9</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="61"/>
-      <c r="C6" s="35" t="s">
+      <c r="B6" s="62"/>
+      <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="14">
         <v>2</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="23">
         <f>F6*Prices!$D$4</f>
         <v>19.98</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="14">
         <v>5</v>
       </c>
-      <c r="I6" s="48">
+      <c r="I6" s="23">
         <f>(H6-F6)*Prices!$D$4</f>
         <v>29.97</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="48">
+      <c r="K6" s="23">
         <f>2*I6/J$4</f>
         <v>59.94</v>
       </c>
-      <c r="L6" s="34" t="s">
+      <c r="L6" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="61"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="62"/>
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="14">
         <v>5</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="23">
         <f>F7*Prices!$D$4</f>
         <v>49.95</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="14">
         <v>25</v>
       </c>
-      <c r="I7" s="48">
+      <c r="I7" s="23">
         <f>(H7-F7)*Prices!$D$4</f>
         <v>199.8</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="48">
+      <c r="K7" s="23">
         <f>2*I7/J$4</f>
         <v>399.6</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="61"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="23"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="61"/>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="62"/>
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="22">
         <f>D9*Prices!D8</f>
         <v>39.96</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="14">
         <v>9</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="23">
         <f>((F9-D9)*Prices!$D$4)/$F$4</f>
         <v>24.975000000000001</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="14">
         <v>49</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="23">
         <f>(H9-F9)*Prices!$D$4</f>
         <v>399.6</v>
       </c>
-      <c r="J9" s="33" t="s">
+      <c r="J9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="48">
+      <c r="K9" s="23">
         <f>2*I9/J$4</f>
         <v>799.2</v>
       </c>
-      <c r="L9" s="20"/>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="61"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="62"/>
+      <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="7">
         <v>9</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="22">
         <f>D10*Prices!D9</f>
         <v>17.91</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="14">
         <v>19</v>
       </c>
-      <c r="G10" s="48">
+      <c r="G10" s="23">
         <f>((F10-D10)*Prices!$D$4)/$F$4</f>
         <v>49.95</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="23">
         <f>(F10*Prices!$D$4)/H$4</f>
         <v>94.905000000000001</v>
       </c>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="48">
+      <c r="K10" s="23">
         <f>2*I10/J$4</f>
         <v>189.81</v>
       </c>
-      <c r="L10" s="20"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="61"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="62"/>
+      <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="7">
         <v>49</v>
       </c>
-      <c r="E11" s="47">
+      <c r="E11" s="22">
         <f>D11*Prices!D10</f>
         <v>48.51</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="14">
         <v>99</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="23">
         <f>((F11-D11)*Prices!$D$4)/$F$4</f>
         <v>249.75</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="H11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="48">
+      <c r="I11" s="23">
         <f>(F11*Prices!$D$4)/H$4</f>
         <v>494.505</v>
       </c>
-      <c r="J11" s="33" t="s">
+      <c r="J11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="48">
+      <c r="K11" s="23">
         <f>2*I11/J$4</f>
         <v>989.01</v>
       </c>
-      <c r="L11" s="20"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="61"/>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="62"/>
+      <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="7">
         <v>49</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="22">
         <f>D12*Prices!D11</f>
         <v>4.41</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="23">
         <f>(D12*Prices!$D$4)/F$4</f>
         <v>244.755</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="48">
+      <c r="I12" s="23">
         <f>(D12*Prices!$D$4*2)/H$4</f>
         <v>489.51</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="J12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="48">
+      <c r="K12" s="23">
         <f>2*I12/J$4</f>
         <v>979.02</v>
       </c>
-      <c r="L12" s="20"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="61"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="23"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="39"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="61"/>
-      <c r="C14" s="15" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="47">
+      <c r="E14" s="22">
         <f>Prices!E14</f>
         <v>2.99</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="23">
         <f>Prices!$E$15</f>
         <v>5.99</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="23">
         <f>Prices!$E$15</f>
         <v>5.99</v>
       </c>
-      <c r="J14" s="33" t="s">
+      <c r="J14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="48">
+      <c r="K14" s="23">
         <f>Prices!$E$16</f>
         <v>9.99</v>
       </c>
-      <c r="L14" s="20"/>
+      <c r="L14" s="8"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="61"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="27"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="30"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="62"/>
-      <c r="C16" s="36" t="s">
+      <c r="B16" s="63"/>
+      <c r="C16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="14">
         <v>1</v>
       </c>
-      <c r="G16" s="48">
+      <c r="G16" s="23">
         <f>F16*Prices!$D$18</f>
         <v>4.99</v>
       </c>
-      <c r="H16" s="33">
+      <c r="H16" s="14">
         <v>5</v>
       </c>
-      <c r="I16" s="48">
+      <c r="I16" s="23">
         <f>H16*Prices!$D$18</f>
         <v>24.950000000000003</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="J16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="48">
+      <c r="K16" s="23">
         <f>2*I16/J$4</f>
         <v>49.900000000000006</v>
       </c>
-      <c r="L16" s="34"/>
+      <c r="L16" s="15"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="44">
         <f>SUM(E9:E12,E14)</f>
         <v>113.77999999999999</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="49">
+      <c r="E18" s="40"/>
+      <c r="F18" s="59">
         <f>SUM(G5:G16)</f>
         <v>680.31</v>
       </c>
-      <c r="G18" s="50"/>
-      <c r="H18" s="49">
+      <c r="G18" s="60"/>
+      <c r="H18" s="59">
         <f>SUM(I5:I16)</f>
         <v>1789.18</v>
       </c>
-      <c r="I18" s="50"/>
-      <c r="J18" s="49">
+      <c r="I18" s="60"/>
+      <c r="J18" s="59">
         <f>SUM(K5:K16)</f>
         <v>3576.37</v>
       </c>
-      <c r="K18" s="50"/>
-      <c r="L18" s="20"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="8"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="69">
+      <c r="D19" s="66">
         <v>99.99</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="49">
+      <c r="E19" s="67"/>
+      <c r="F19" s="59">
         <v>699.99</v>
       </c>
-      <c r="G19" s="50"/>
-      <c r="H19" s="49">
+      <c r="G19" s="60"/>
+      <c r="H19" s="59">
         <v>1799.99</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="49">
+      <c r="I19" s="60"/>
+      <c r="J19" s="59">
         <v>3599.99</v>
       </c>
-      <c r="K19" s="50"/>
-      <c r="L19" s="20"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="8"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="56"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="70"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="59"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="D15:L15"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="C22:L22"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="J18:K18"/>
@@ -2105,19 +2118,9 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="C21:L21"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D8:L8"/>
-    <mergeCell ref="D13:L13"/>
-    <mergeCell ref="D15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed payment warning message for [settings | granularity] to credit card form.
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795F1212-C402-4125-8448-6ACA5ABD449F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5542EA22-8D23-4282-910E-5F4F38264F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Package pricing" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -591,12 +592,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -627,6 +622,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -636,11 +643,26 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -656,27 +678,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C75CBC2-A4B4-4CDB-9F64-6654769FA256}">
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,10 +1120,10 @@
         <v>6</v>
       </c>
       <c r="D8" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7">
         <v>5</v>
@@ -1324,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8890EB03-9831-4A84-BAA4-07E57C463030}">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,17 +1340,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="46" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="19" t="s">
         <v>24</v>
       </c>
@@ -1367,10 +1368,10 @@
       <c r="C4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="54">
         <v>9.99</v>
       </c>
-      <c r="E4" s="44"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
@@ -1380,10 +1381,10 @@
       <c r="C5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="54">
         <v>5.99</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
@@ -1393,17 +1394,17 @@
       <c r="C6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="54">
         <v>2.99</v>
       </c>
-      <c r="E6" s="44"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="42"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="30"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1411,10 +1412,10 @@
       <c r="C8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="54">
         <v>9.99</v>
       </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="12" t="s">
         <v>34</v>
       </c>
@@ -1424,10 +1425,10 @@
       <c r="C9" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="54">
         <v>1.99</v>
       </c>
-      <c r="E9" s="44"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="12" t="s">
         <v>35</v>
       </c>
@@ -1437,10 +1438,10 @@
       <c r="C10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="54">
         <v>0.99</v>
       </c>
-      <c r="E10" s="44"/>
+      <c r="E10" s="54"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1448,10 +1449,10 @@
       <c r="C11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="54">
         <v>0.09</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="54"/>
       <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
@@ -1459,13 +1460,13 @@
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="42"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="52"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="29"/>
       <c r="F12" s="30"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="47" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1480,7 +1481,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
-      <c r="C14" s="50"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="7" t="s">
         <v>26</v>
       </c>
@@ -1493,7 +1494,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
-      <c r="C15" s="50"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="7" t="s">
         <v>27</v>
       </c>
@@ -1506,7 +1507,7 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="42"/>
-      <c r="C16" s="51"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="7" t="s">
         <v>30</v>
       </c>
@@ -1520,7 +1521,7 @@
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="45"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="29"/>
       <c r="F17" s="30"/>
     </row>
@@ -1529,10 +1530,10 @@
       <c r="C18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="44">
+      <c r="D18" s="54">
         <v>4.99</v>
       </c>
-      <c r="E18" s="44">
+      <c r="E18" s="54">
         <v>4.99</v>
       </c>
       <c r="F18" s="12" t="s">
@@ -1590,22 +1591,22 @@
     <row r="2" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="71" t="s">
+      <c r="E2" s="67"/>
+      <c r="F2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="71" t="s">
+      <c r="G2" s="67"/>
+      <c r="H2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="72"/>
-      <c r="J2" s="71" t="s">
+      <c r="I2" s="67"/>
+      <c r="J2" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="72"/>
+      <c r="K2" s="67"/>
       <c r="L2" s="21" t="s">
         <v>10</v>
       </c>
@@ -1642,30 +1643,30 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="68" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="64">
+      <c r="D4" s="71"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="71">
         <v>2</v>
       </c>
-      <c r="G4" s="65"/>
-      <c r="H4" s="64">
+      <c r="G4" s="72"/>
+      <c r="H4" s="71">
         <v>2</v>
       </c>
-      <c r="I4" s="65"/>
-      <c r="J4" s="64">
+      <c r="I4" s="72"/>
+      <c r="J4" s="71">
         <v>1</v>
       </c>
-      <c r="K4" s="65"/>
+      <c r="K4" s="72"/>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="62"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1701,7 +1702,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="62"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
@@ -1737,7 +1738,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="62"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1773,7 +1774,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="62"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="3"/>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
@@ -1786,7 +1787,7 @@
       <c r="L8" s="39"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="62"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1821,7 +1822,7 @@
       <c r="L9" s="8"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="62"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1856,7 +1857,7 @@
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="62"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1891,7 +1892,7 @@
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="62"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
@@ -1926,7 +1927,7 @@
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="62"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="3"/>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
@@ -1939,7 +1940,7 @@
       <c r="L13" s="39"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="62"/>
+      <c r="B14" s="69"/>
       <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
@@ -1974,7 +1975,7 @@
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="62"/>
+      <c r="B15" s="69"/>
       <c r="C15" s="3"/>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
@@ -1987,7 +1988,7 @@
       <c r="L15" s="30"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="63"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="17" t="s">
         <v>21</v>
       </c>
@@ -2024,77 +2025,77 @@
       <c r="C18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="44">
+      <c r="D18" s="54">
         <f>SUM(E9:E12,E14)</f>
         <v>113.77999999999999</v>
       </c>
       <c r="E18" s="40"/>
-      <c r="F18" s="59">
+      <c r="F18" s="56">
         <f>SUM(G5:G16)</f>
         <v>680.31</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="59">
+      <c r="G18" s="57"/>
+      <c r="H18" s="56">
         <f>SUM(I5:I16)</f>
         <v>1789.18</v>
       </c>
-      <c r="I18" s="60"/>
-      <c r="J18" s="59">
+      <c r="I18" s="57"/>
+      <c r="J18" s="56">
         <f>SUM(K5:K16)</f>
         <v>3576.37</v>
       </c>
-      <c r="K18" s="60"/>
+      <c r="K18" s="57"/>
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="66">
+      <c r="D19" s="61">
         <v>99.99</v>
       </c>
-      <c r="E19" s="67"/>
-      <c r="F19" s="59">
+      <c r="E19" s="62"/>
+      <c r="F19" s="56">
         <v>699.99</v>
       </c>
-      <c r="G19" s="60"/>
-      <c r="H19" s="59">
+      <c r="G19" s="57"/>
+      <c r="H19" s="56">
         <v>1799.99</v>
       </c>
-      <c r="I19" s="60"/>
-      <c r="J19" s="59">
+      <c r="I19" s="57"/>
+      <c r="J19" s="56">
         <v>3599.99</v>
       </c>
-      <c r="K19" s="60"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="8"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="68" t="s">
+      <c r="C21" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="70"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="65"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="58"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -2106,16 +2107,16 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B4:B16"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="C22:L22"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B4:B16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="C21:L21"/>
     <mergeCell ref="F19:G19"/>

</xml_diff>